<commit_message>
Unit-Tests done, Grobschliff done
</commit_message>
<xml_diff>
--- a/repos/Checklist.xlsx
+++ b/repos/Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FH\FHTW-Sem-3-SWE\repos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDB5E6B-EBD0-4B40-862F-D60B8E277FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390E32D9-F96D-4CA3-9A61-E92D6A070511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
   </bookViews>
@@ -179,7 +179,7 @@
     <t>Describes design</t>
   </si>
   <si>
-    <t>anscheinend</t>
+    <t>nix</t>
   </si>
 </sst>
 </file>
@@ -248,7 +248,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -273,6 +273,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -286,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -299,7 +305,8 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -634,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D58600B0-3567-4A3D-A785-925E0537D06D}">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47:E52"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -701,9 +708,6 @@
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
@@ -742,7 +746,7 @@
         <v>12</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -830,7 +834,7 @@
       <c r="A26" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="13">
         <v>0</v>
       </c>
       <c r="C26" s="6">
@@ -897,10 +901,13 @@
       <c r="A33" s="6" t="s">
         <v>28</v>
       </c>
+      <c r="B33" s="13">
+        <v>0</v>
+      </c>
       <c r="C33" s="6">
         <v>1</v>
       </c>
-      <c r="E33" s="11"/>
+      <c r="E33" s="10"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
@@ -912,7 +919,7 @@
       <c r="C34" s="6">
         <v>2</v>
       </c>
-      <c r="E34" s="11"/>
+      <c r="E34" s="10"/>
     </row>
     <row r="36" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
@@ -959,25 +966,33 @@
       <c r="A41" s="6" t="s">
         <v>34</v>
       </c>
+      <c r="B41">
+        <v>5</v>
+      </c>
       <c r="C41" s="6">
         <v>5</v>
       </c>
-      <c r="E41" s="11"/>
+      <c r="E41" s="10"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
         <v>35</v>
       </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
       <c r="C42" s="6">
         <v>3</v>
       </c>
-      <c r="E42" s="11"/>
+      <c r="E42" s="10"/>
     </row>
     <row r="44" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B44"/>
+      <c r="B44" t="s">
+        <v>47</v>
+      </c>
       <c r="C44" s="6"/>
       <c r="E44" s="12"/>
     </row>
@@ -1048,7 +1063,7 @@
       </c>
       <c r="B54" s="2">
         <f>IF(MIN(B9:B16)=1,SUM(B21:B52),0)</f>
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="C54" s="2">
         <f>SUM(C21:C52)</f>
@@ -1067,21 +1082,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100495F7CC252815B47896F98900E10984C" ma:contentTypeVersion="2" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="afe1b3b164495dc81fdbcdcad6ec8b68">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="207955a2-a3fc-4582-b2ea-e4c7d1fb6048" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b6a42bf87c3f8727d31c248fc1697f6" ns2:_="">
     <xsd:import namespace="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
@@ -1213,10 +1213,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B871BF9-5772-4B74-B6DF-7878EF29873D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0824ED0-660A-437B-A039-7835C5DD208D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1238,19 +1263,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0824ED0-660A-437B-A039-7835C5DD208D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B871BF9-5772-4B74-B6DF-7878EF29873D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Dateien verschoben / aufgeräumt
</commit_message>
<xml_diff>
--- a/repos/Checklist.xlsx
+++ b/repos/Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FH\FHTW-Sem-3-SWE\repos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390E32D9-F96D-4CA3-9A61-E92D6A070511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7D4416-1C29-4A45-A70E-C0B900C99137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
   </bookViews>
@@ -641,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D58600B0-3567-4A3D-A785-925E0537D06D}">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -925,7 +925,9 @@
       <c r="A36" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B36"/>
+      <c r="B36">
+        <v>3</v>
+      </c>
       <c r="C36" s="6">
         <v>3</v>
       </c>
@@ -1063,7 +1065,7 @@
       </c>
       <c r="B54" s="2">
         <f>IF(MIN(B9:B16)=1,SUM(B21:B52),0)</f>
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C54" s="2">
         <f>SUM(C21:C52)</f>
@@ -1082,6 +1084,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100495F7CC252815B47896F98900E10984C" ma:contentTypeVersion="2" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="afe1b3b164495dc81fdbcdcad6ec8b68">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="207955a2-a3fc-4582-b2ea-e4c7d1fb6048" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b6a42bf87c3f8727d31c248fc1697f6" ns2:_="">
     <xsd:import namespace="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
@@ -1213,35 +1230,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0824ED0-660A-437B-A039-7835C5DD208D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B871BF9-5772-4B74-B6DF-7878EF29873D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1263,9 +1255,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B871BF9-5772-4B74-B6DF-7878EF29873D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0824ED0-660A-437B-A039-7835C5DD208D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>